<commit_message>
Add Modifer order testcases
</commit_message>
<xml_diff>
--- a/test-report.xlsx
+++ b/test-report.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="185">
   <si>
     <t xml:space="preserve">Passed</t>
   </si>
@@ -158,10 +158,7 @@
     <t xml:space="preserve">FUNC 006</t>
   </si>
   <si>
-    <t xml:space="preserve">Add store to Food Court when not logged in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go to Manage Food Court page</t>
+    <t xml:space="preserve">Go toManager Food Court page when not logged in</t>
   </si>
   <si>
     <t xml:space="preserve">Succesfull</t>
@@ -170,54 +167,60 @@
     <t xml:space="preserve">Đỗ Lê Quang Trung</t>
   </si>
   <si>
+    <t xml:space="preserve">Click "Quản lý cửa hàng"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notify "Please login to see this page"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to Manager Food Court page when logged in with customer account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notify " Bạn không có quyền thực hiện chức năng này"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add store to Food Court when logged in with food court manager account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Succesfull if already have an account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New store will add to database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to Manager Food Court page</t>
+  </si>
+  <si>
     <t xml:space="preserve">Click "Thêm cửa hàng"</t>
   </si>
   <si>
-    <t xml:space="preserve">notify "Please login to see this page"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete store from Food Court when not logged in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go to Manager page</t>
+    <t xml:space="preserve">Go to fill out form page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Add"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete store from Food Court when logged in with food court manager account (accept request)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete store from database</t>
   </si>
   <si>
     <t xml:space="preserve">Click "Xóa cửa hàng"</t>
   </si>
   <si>
-    <t xml:space="preserve">FUNC 008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add store to Food Court when logged in with food court manager account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Succesfull if already have an account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New store will add to database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go to fill out form page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click "Add"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete store from Food Court when logged in with food court manager account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete store from database</t>
-  </si>
-  <si>
     <t xml:space="preserve">notify " Bạn có chắc chắn xóa cửa hàng"</t>
   </si>
   <si>
@@ -227,16 +230,28 @@
     <t xml:space="preserve">FUNC 010</t>
   </si>
   <si>
-    <t xml:space="preserve">Add store to Food Court when logged in with customer account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notify " Bạn không có quyền thực hiện chức năng này"</t>
+    <t xml:space="preserve">Delete store from Food Court when logged in with food court manager account (cancel request)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database change nothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Cancel"</t>
   </si>
   <si>
     <t xml:space="preserve">FUNC 011</t>
   </si>
   <si>
-    <t xml:space="preserve">Delete store from Food Court when logged in with customer account</t>
+    <t xml:space="preserve">View food court report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show business situation of food court and every store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unavailable, Not run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Xem báo cáo kinh doanh"</t>
   </si>
   <si>
     <t xml:space="preserve">Modify cart</t>
@@ -329,10 +344,216 @@
     <t xml:space="preserve">notify "Thất bại"</t>
   </si>
   <si>
+    <t xml:space="preserve">View order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View order when not logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to order page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lê Đức Huy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View order when  logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to order page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show list of paid bills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View order when  logged in (in detail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show all information about the order : order id, customer name, date, dishes, price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose an order </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search dish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on search bar and enter keyword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show list of dishes which has a keyword. If a dish has a keyword don't exist, the result return blank </t>
+  </si>
+  <si>
+    <t xml:space="preserve">press "Enter"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The search engine will returns with the result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search dish with special symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on search bar and enter keyword with special symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The result return blank </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search dish when loggin and not loggin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The results are the same </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change order status when not logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to manage order page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access to change order status page. Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose order need change status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change status of an order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change order status when logged in with cook account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update order's status in order page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order's status had not been changed. Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notify "Đã cập nhật trạng thái"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change order status when logged in with customer account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order's status had not been changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notify " Bạn không có quyền thực hiện chức năng này "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the history button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User’s personal bought history is shown along with information: dish name, date and time bought, store name, prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lê Trung Đan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rating function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate dish among search results when user has not bought the dish already</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selected target dish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unable to rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rating button unavailable, Not completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select “đánh giá”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button greyed out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate dish among search results when user has bought the dish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on target dish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database updated.
+Refresh average rating and comments.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rating button unavailable, Not run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “Đánh giá”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose from 1 to 5 stars and optionally comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated stars glow up
+Interactively present comment box afterwards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “Hoàn thành”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC 031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate dish available in user history</t>
+  </si>
+  <si>
     <t xml:space="preserve">External payment</t>
   </si>
   <si>
-    <t xml:space="preserve">FUNC 019</t>
+    <t xml:space="preserve">FUNC 032</t>
   </si>
   <si>
     <t xml:space="preserve">Choose an external payment service</t>
@@ -344,13 +565,7 @@
     <t xml:space="preserve">Redirected to 3rd-party’s website</t>
   </si>
   <si>
-    <t xml:space="preserve">Unavailable, Not run</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lê Trung Đan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 020</t>
+    <t xml:space="preserve">FUNC 033</t>
   </si>
   <si>
     <t xml:space="preserve">Perform payment when the external account has enough money</t>
@@ -363,168 +578,13 @@
 Send orders to stores</t>
   </si>
   <si>
-    <t xml:space="preserve">FUNC 021</t>
+    <t xml:space="preserve">FUNC 034</t>
   </si>
   <si>
     <t xml:space="preserve">Perform payment when the external account doesn’t have enough money</t>
   </si>
   <si>
     <t xml:space="preserve">Request recharge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">View order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">View order when not logged in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go to order page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lê Đức Huy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">View order when  logged in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go to order page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show list of paid bills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">View order when  logged in (in detail)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show all information about the order : order id, customer name, date, dishes, price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose an order </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search dish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on search bar and enter keyword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show list of dishes which has a keyword. If a dish has a keyword don't exist, the result return blank </t>
-  </si>
-  <si>
-    <t xml:space="preserve">press "Enter"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The search engine will returns with the result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search dish with special symbol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on search bar and enter keyword with special symbol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The result return blank </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search dish when loggin and not loggin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The results are the same </t>
-  </si>
-  <si>
-    <t xml:space="preserve">User history</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show history</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on the history button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User’s personal bought history is shown along with information: dish name, date and time bought, store name, prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rating function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate dish among search results when user has not bought the dish already</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selected target dish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unable to rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rating button unavailable, Not completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select “đánh giá”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button greyed out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate dish among search results when user has bought the dish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on target dish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database updated.
-Refresh average rating and comments.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rating button unavailable, Not run</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on “Đánh giá”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose from 1 to 5 stars and optionally comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated stars glow up
-Interactively present comment box afterwards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on “Hoàn thành”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC 031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate dish available in user history</t>
   </si>
 </sst>
 </file>
@@ -539,7 +599,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -561,7 +621,8 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -641,20 +702,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -734,35 +795,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I77" activeCellId="0" sqref="I77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.9"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="8.8"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="n">
         <f aca="false">H5-SUM(H2:H4)</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
@@ -770,20 +831,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -791,7 +852,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -832,7 +893,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -858,7 +919,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -891,7 +952,7 @@
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -908,7 +969,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -922,7 +983,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -936,7 +997,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
         <v>28</v>
@@ -958,7 +1019,7 @@
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -972,7 +1033,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -986,7 +1047,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>34</v>
@@ -1008,7 +1069,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1036,7 +1097,7 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="40.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="40.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="2" t="s">
         <v>36</v>
@@ -1069,10 +1130,10 @@
         <v>43</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>18</v>
@@ -1081,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1089,31 +1150,31 @@
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="31.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>0</v>
@@ -1125,10 +1186,10 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1137,45 +1198,45 @@
     <row r="25" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="E25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="F25" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>0</v>
       </c>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>58</v>
@@ -1192,7 +1253,7 @@
         <v>59</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1207,10 +1268,10 @@
         <v>61</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>62</v>
@@ -1220,15 +1281,15 @@
       </c>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -1239,10 +1300,10 @@
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -1253,10 +1314,10 @@
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -1265,448 +1326,420 @@
     <row r="33" customFormat="false" ht="28.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>0</v>
       </c>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
-      <c r="B35" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
       <c r="D35" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>0</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
+    <row r="37" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F37" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G37" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="41.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="1" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
-      <c r="H39" s="6"/>
+      <c r="H39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5"/>
+      <c r="A40" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="B40" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41" customFormat="false" ht="35.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H40" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="6"/>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H43" s="6"/>
-    </row>
-    <row r="44" customFormat="false" ht="29.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="35.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
-      <c r="H44" s="6"/>
-    </row>
-    <row r="45" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
-      <c r="B45" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H45" s="6"/>
-    </row>
-    <row r="46" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C46" s="5"/>
       <c r="D46" s="1" t="s">
         <v>88</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="6"/>
-    </row>
-    <row r="47" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="29.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C47" s="5" t="s">
+      <c r="E47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="5" t="s">
+      <c r="C48" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H47" s="6"/>
-    </row>
-    <row r="48" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="6"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="5"/>
       <c r="B49" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="E49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F49" s="6" t="s">
+      <c r="B50" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="D50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H49" s="6"/>
-    </row>
-    <row r="50" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5" t="s">
+      <c r="E51" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F51" s="5" t="s">
+      <c r="C52" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F54" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G51" s="5" t="s">
+      <c r="G54" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H51" s="6"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="6"/>
-    </row>
-    <row r="53" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F53" s="6" t="s">
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G53" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5"/>
-      <c r="B54" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5"/>
-      <c r="B55" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>105</v>
-      </c>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
       <c r="H55" s="5"/>
     </row>
     <row r="56" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>18</v>
@@ -1714,237 +1747,225 @@
       <c r="G56" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H56" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H56" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5"/>
       <c r="B57" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H57" s="6"/>
+      <c r="H57" s="5"/>
     </row>
     <row r="58" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H58" s="6"/>
+      <c r="H58" s="5"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
-      <c r="H59" s="6"/>
+      <c r="H59" s="5"/>
     </row>
     <row r="60" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H60" s="6"/>
-    </row>
-    <row r="61" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
-      <c r="H61" s="6"/>
+      <c r="H61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="41.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>137</v>
+        <v>44</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H62" s="6"/>
-    </row>
-    <row r="63" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F63" s="9"/>
+        <v>124</v>
+      </c>
+      <c r="F63" s="7"/>
       <c r="G63" s="5"/>
-      <c r="H63" s="6"/>
+      <c r="H63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>139</v>
+        <v>129</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H64" s="6"/>
-    </row>
-    <row r="65" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
-      <c r="C65" s="6"/>
+      <c r="C65" s="5"/>
       <c r="D65" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
-      <c r="H65" s="6"/>
-    </row>
-    <row r="66" customFormat="false" ht="77.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" customFormat="false" ht="77.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>148</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
       <c r="D67" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="H67" s="6"/>
-    </row>
-    <row r="68" customFormat="false" ht="51.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" customFormat="false" ht="51.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="5"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
       <c r="D68" s="1" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>153</v>
+        <v>47</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
@@ -1952,134 +1973,367 @@
     </row>
     <row r="69" customFormat="false" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="5"/>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="B76" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="C76" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F69" s="6" t="s">
+      <c r="D76" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G69" s="10" t="s">
+      <c r="E76" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F76" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="H69" s="6"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="1" t="s">
+      <c r="G76" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F70" s="6"/>
-      <c r="G70" s="10"/>
-      <c r="H70" s="6"/>
-    </row>
-    <row r="71" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="1" t="s">
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E77" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F71" s="6"/>
-      <c r="G71" s="10"/>
-      <c r="H71" s="6"/>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="1" t="s">
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F72" s="6"/>
-      <c r="G72" s="10"/>
-      <c r="H72" s="6"/>
-    </row>
-    <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5"/>
-      <c r="B73" s="6" t="s">
+      <c r="C78" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="D78" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G73" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="H73" s="6"/>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-    </row>
-    <row r="75" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="6"/>
-      <c r="D75" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5"/>
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-    </row>
+      <c r="E78" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F79" s="5"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F80" s="5"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F81" s="5"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" customFormat="false" ht="41.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G86" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="5"/>
+      <c r="B87" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="5"/>
+      <c r="B88" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="G88" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" customFormat="false" ht="41.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="117">
+  <mergeCells count="129">
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -2105,12 +2359,12 @@
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="G17:G19"/>
-    <mergeCell ref="A21:A36"/>
+    <mergeCell ref="A21:A39"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H36"/>
+    <mergeCell ref="H21:H39"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="F23:F24"/>
@@ -2123,49 +2377,47 @@
     <mergeCell ref="C29:C32"/>
     <mergeCell ref="F29:F32"/>
     <mergeCell ref="G29:G32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="G33:G36"/>
     <mergeCell ref="B37:B39"/>
     <mergeCell ref="C37:C39"/>
     <mergeCell ref="F37:F39"/>
     <mergeCell ref="G37:G39"/>
-    <mergeCell ref="H37:H52"/>
+    <mergeCell ref="A40:A49"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="C40:C42"/>
     <mergeCell ref="F40:F42"/>
     <mergeCell ref="G40:G42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="H53:H55"/>
+    <mergeCell ref="H40:H55"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="A50:A55"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
     <mergeCell ref="A56:A59"/>
-    <mergeCell ref="H56:H65"/>
+    <mergeCell ref="H56:H74"/>
     <mergeCell ref="B58:B59"/>
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="F58:F59"/>
@@ -2183,20 +2435,34 @@
     <mergeCell ref="C64:C65"/>
     <mergeCell ref="F64:F65"/>
     <mergeCell ref="G64:G65"/>
-    <mergeCell ref="H66:H76"/>
-    <mergeCell ref="A67:A76"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="B69:B72"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="F69:F72"/>
-    <mergeCell ref="G69:G72"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="F73:F76"/>
-    <mergeCell ref="G73:G76"/>
+    <mergeCell ref="A66:A74"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="F66:F68"/>
+    <mergeCell ref="G66:G68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="F69:F71"/>
+    <mergeCell ref="G69:G71"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="F72:F74"/>
+    <mergeCell ref="G72:G74"/>
+    <mergeCell ref="H75:H88"/>
+    <mergeCell ref="A76:A85"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="G76:G77"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="G78:G81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="F82:F85"/>
+    <mergeCell ref="G82:G85"/>
+    <mergeCell ref="A86:A88"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2219,7 +2485,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2242,7 +2508,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Fix typos in test report
</commit_message>
<xml_diff>
--- a/test-report.xlsx
+++ b/test-report.xlsx
@@ -92,7 +92,7 @@
   </si>
   <si>
     <t xml:space="preserve">Account name showed,
-Passedword hidden</t>
+Password hidden</t>
   </si>
   <si>
     <t xml:space="preserve">FUNC 002</t>
@@ -161,7 +161,7 @@
     <t xml:space="preserve">Go toManager Food Court page when not logged in</t>
   </si>
   <si>
-    <t xml:space="preserve">Succesfull</t>
+    <t xml:space="preserve">Successful</t>
   </si>
   <si>
     <t xml:space="preserve">Đỗ Lê Quang Trung</t>
@@ -191,7 +191,7 @@
     <t xml:space="preserve">Login</t>
   </si>
   <si>
-    <t xml:space="preserve">Succesfull if already have an account</t>
+    <t xml:space="preserve">Successful if already have an account</t>
   </si>
   <si>
     <t xml:space="preserve">New store will add to database</t>
@@ -395,7 +395,25 @@
     <t xml:space="preserve">Click on search bar and enter keyword</t>
   </si>
   <si>
-    <t xml:space="preserve">Show list of dishes which has a keyword. If a dish has a keyword don't exist, the result return blank </t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Show list of dishes which has a keyword. If there is no such a dish, the return blank </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">result</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">press "Enter"</t>
@@ -497,7 +515,7 @@
     <t xml:space="preserve">FUNC 029</t>
   </si>
   <si>
-    <t xml:space="preserve">Rate dish among search results when user has not bought the dish already</t>
+    <t xml:space="preserve">Rate dishes among search results when user has not bought the dish already</t>
   </si>
   <si>
     <t xml:space="preserve">Selected target dish</t>
@@ -518,7 +536,7 @@
     <t xml:space="preserve">FUNC 030</t>
   </si>
   <si>
-    <t xml:space="preserve">Rate dish among search results when user has bought the dish</t>
+    <t xml:space="preserve">Rate dishes among search results when user has bought the dish</t>
   </si>
   <si>
     <t xml:space="preserve">Click on target dish</t>
@@ -547,7 +565,7 @@
     <t xml:space="preserve">FUNC 031</t>
   </si>
   <si>
-    <t xml:space="preserve">Rate dish available in user history</t>
+    <t xml:space="preserve">Rate dishes available in user history</t>
   </si>
   <si>
     <t xml:space="preserve">External payment</t>
@@ -594,7 +612,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -614,6 +632,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
     </font>
@@ -706,11 +730,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -797,8 +821,8 @@
   </sheetPr>
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I77" activeCellId="0" sqref="I77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -919,7 +943,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2043,7 +2067,7 @@
       </c>
       <c r="H72" s="5"/>
     </row>
-    <row r="73" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
@@ -2071,7 +2095,7 @@
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
     </row>
-    <row r="75" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="86.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
         <v>148</v>
       </c>
@@ -2097,7 +2121,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
         <v>154</v>
       </c>
@@ -2135,7 +2159,7 @@
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="5"/>
       <c r="B78" s="5" t="s">
         <v>162</v>
@@ -2199,7 +2223,7 @@
       <c r="G81" s="9"/>
       <c r="H81" s="5"/>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="5"/>
       <c r="B82" s="5" t="s">
         <v>171</v>

</xml_diff>